<commit_message>
finaly found the problem, good thing i looked at the original artical
</commit_message>
<xml_diff>
--- a/starting with data/excel files/their_data.xlsx
+++ b/starting with data/excel files/their_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailtauacil-my.sharepoint.com/personal/jy1_mail_tau_ac_il/Documents/Desktop/אוניברסיטה/אסטרו נודר/פרויקט קיץ/התחלה של קוד/astro_summer_project/starting with data/excel files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_46D1A390872734C6CF6958B94CB7F8EC7452E42D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06D89399-8C44-4E76-BE49-E3B48DB8793F}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_46D1A390872734C6CF6958B94CB7F8EC7452E42D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA36E9E2-7575-4A85-8459-4ABAAA4133D6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1335,7 +1335,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" activeCellId="2" sqref="C1:C1048576 E1:E1048576 F1:F1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1859,7 +1859,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
well, SW16 does not fit well on the data. moving on to another model
</commit_message>
<xml_diff>
--- a/starting with data/excel files/their_data.xlsx
+++ b/starting with data/excel files/their_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailtauacil-my.sharepoint.com/personal/jy1_mail_tau_ac_il/Documents/Desktop/אוניברסיטה/אסטרו נודר/פרויקט קיץ/התחלה של קוד/astro_summer_project/starting with data/excel files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="11_46D1A390872734C6CF6958B94CB7F8EC7452E42D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D41A92F-049E-41AB-B444-908E516A93AA}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="11_46D1A390872734C6CF6958B94CB7F8EC7452E42D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B89FDB43-E43E-4408-8998-649B44ADAF8C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="after beaning" sheetId="1" r:id="rId1"/>
@@ -964,7 +964,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -991,12 +991,6 @@
       <color rgb="FF6897BB"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="177"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2129,10 +2123,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0505C6EC-8959-4512-9AB0-5FB33F120081}">
-  <dimension ref="A1:F114"/>
+  <dimension ref="A1:J114"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2717,7 +2711,7 @@
       </c>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" ht="26.4" customHeight="1">
+    <row r="33" spans="1:10" ht="26.4" customHeight="1">
       <c r="A33" s="2">
         <v>33</v>
       </c>
@@ -2735,7 +2729,7 @@
       </c>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" ht="26.4" customHeight="1">
+    <row r="34" spans="1:10" ht="26.4" customHeight="1">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -2753,7 +2747,7 @@
       </c>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:6" ht="26.4" customHeight="1">
+    <row r="35" spans="1:10" ht="26.4" customHeight="1">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -2771,7 +2765,7 @@
       </c>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="1:6" ht="26.4" customHeight="1">
+    <row r="36" spans="1:10" ht="26.4" customHeight="1">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -2789,7 +2783,7 @@
       </c>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:6" ht="26.4" customHeight="1">
+    <row r="37" spans="1:10" ht="26.4" customHeight="1">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -2807,7 +2801,7 @@
       </c>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="1:6" ht="26.4" customHeight="1">
+    <row r="38" spans="1:10" ht="26.4" customHeight="1">
       <c r="A38" s="2">
         <v>36</v>
       </c>
@@ -2825,7 +2819,7 @@
       </c>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="1:6" ht="26.4" customHeight="1">
+    <row r="39" spans="1:10" ht="26.4" customHeight="1">
       <c r="A39" s="2">
         <v>37</v>
       </c>
@@ -2843,7 +2837,7 @@
       </c>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="1:6" ht="26.4" customHeight="1">
+    <row r="40" spans="1:10" ht="26.4" customHeight="1">
       <c r="A40" s="2">
         <v>38</v>
       </c>
@@ -2861,7 +2855,7 @@
       </c>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="1:6" ht="26.4" customHeight="1">
+    <row r="41" spans="1:10" ht="26.4" customHeight="1">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -2879,7 +2873,7 @@
       </c>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:6" ht="26.4" customHeight="1">
+    <row r="42" spans="1:10" ht="26.4" customHeight="1">
       <c r="A42" s="2">
         <v>40</v>
       </c>
@@ -2899,7 +2893,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="26.4" customHeight="1">
+    <row r="43" spans="1:10" ht="26.4" customHeight="1">
       <c r="A43" s="2" t="s">
         <v>10</v>
       </c>
@@ -2918,8 +2912,12 @@
       <c r="F43" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="26.4" customHeight="1">
+      <c r="J43">
+        <f>B43-B42</f>
+        <v>3.2728870000000021E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="26.4" customHeight="1">
       <c r="A44" s="2" t="s">
         <v>11</v>
       </c>
@@ -2939,7 +2937,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="26.4" customHeight="1">
+    <row r="45" spans="1:10" ht="26.4" customHeight="1">
       <c r="A45" s="2" t="s">
         <v>12</v>
       </c>
@@ -2959,7 +2957,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="26.4" customHeight="1">
+    <row r="46" spans="1:10" ht="26.4" customHeight="1">
       <c r="A46" s="2" t="s">
         <v>13</v>
       </c>
@@ -2979,7 +2977,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="26.4" customHeight="1">
+    <row r="47" spans="1:10" ht="26.4" customHeight="1">
       <c r="A47" s="2">
         <v>41</v>
       </c>
@@ -2999,7 +2997,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="26.4" customHeight="1">
+    <row r="48" spans="1:10" ht="26.4" customHeight="1">
       <c r="A48" s="2">
         <v>42</v>
       </c>
@@ -11464,8 +11462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEE5BCB-D257-4E19-8295-AF23EEBA27F3}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>